<commit_message>
Remove wrong holidays date in example 39
</commit_message>
<xml_diff>
--- a/excel-input/39-assign-423-time-marching/39-assign-423-time-marching.xlsx
+++ b/excel-input/39-assign-423-time-marching/39-assign-423-time-marching.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="9"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="expert" sheetId="1" state="visible" r:id="rId3"/>
@@ -2476,7 +2476,7 @@
   </sheetPr>
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -3069,12 +3069,12 @@
         <v>156</v>
       </c>
       <c r="F2" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B2, C2, holiday!A$2:A$500)</f>
-        <v>110</v>
+        <f aca="false">NETWORKDAYS(B2, C2, holiday!A$2:A$499)</f>
+        <v>111</v>
       </c>
       <c r="G2" s="20" t="n">
         <f aca="false">D2/F2</f>
-        <v>0.727272727272727</v>
+        <v>0.720720720720721</v>
       </c>
       <c r="H2" s="21" t="n">
         <f aca="false">_xlfn.FLOOR.MATH(G2, 0.25)</f>
@@ -3115,7 +3115,7 @@
         <v>31</v>
       </c>
       <c r="F3" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B3, C3, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B3, C3, holiday!A$2:A$499)</f>
         <v>21</v>
       </c>
       <c r="G3" s="20" t="n">
@@ -3161,12 +3161,12 @@
         <v>56</v>
       </c>
       <c r="F4" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B4, C4, holiday!A$2:A$500)</f>
-        <v>39</v>
+        <f aca="false">NETWORKDAYS(B4, C4, holiday!A$2:A$499)</f>
+        <v>40</v>
       </c>
       <c r="G4" s="20" t="n">
         <f aca="false">D4/F4</f>
-        <v>0.641025641025641</v>
+        <v>0.625</v>
       </c>
       <c r="H4" s="21" t="n">
         <f aca="false">_xlfn.FLOOR.MATH(G4, 0.25)</f>
@@ -3207,7 +3207,7 @@
         <v>46</v>
       </c>
       <c r="F5" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B5, C5, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B5, C5, holiday!A$2:A$499)</f>
         <v>33</v>
       </c>
       <c r="G5" s="20" t="n">
@@ -3253,7 +3253,7 @@
         <v>18</v>
       </c>
       <c r="F6" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B6, C6, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B6, C6, holiday!A$2:A$499)</f>
         <v>14</v>
       </c>
       <c r="G6" s="20" t="n">
@@ -3299,7 +3299,7 @@
         <v>123</v>
       </c>
       <c r="F7" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B7, C7, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B7, C7, holiday!A$2:A$499)</f>
         <v>86</v>
       </c>
       <c r="G7" s="20" t="n">
@@ -3345,7 +3345,7 @@
         <v>46</v>
       </c>
       <c r="F8" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B8, C8, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B8, C8, holiday!A$2:A$499)</f>
         <v>34</v>
       </c>
       <c r="G8" s="20" t="n">
@@ -3391,7 +3391,7 @@
         <v>11</v>
       </c>
       <c r="F9" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B9, C9, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B9, C9, holiday!A$2:A$499)</f>
         <v>7</v>
       </c>
       <c r="G9" s="20" t="n">
@@ -3437,7 +3437,7 @@
         <v>158</v>
       </c>
       <c r="F10" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B10, C10, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B10, C10, holiday!A$2:A$499)</f>
         <v>113</v>
       </c>
       <c r="G10" s="20" t="n">
@@ -3483,7 +3483,7 @@
         <v>35</v>
       </c>
       <c r="F11" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B11, C11, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B11, C11, holiday!A$2:A$499)</f>
         <v>25</v>
       </c>
       <c r="G11" s="20" t="n">
@@ -3529,7 +3529,7 @@
         <v>20</v>
       </c>
       <c r="F12" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B12, C12, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B12, C12, holiday!A$2:A$499)</f>
         <v>15</v>
       </c>
       <c r="G12" s="20" t="n">
@@ -3575,7 +3575,7 @@
         <v>199</v>
       </c>
       <c r="F13" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B13, C13, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B13, C13, holiday!A$2:A$499)</f>
         <v>142</v>
       </c>
       <c r="G13" s="20" t="n">
@@ -3621,7 +3621,7 @@
         <v>32</v>
       </c>
       <c r="F14" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B14, C14, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B14, C14, holiday!A$2:A$499)</f>
         <v>23</v>
       </c>
       <c r="G14" s="20" t="n">
@@ -3667,12 +3667,12 @@
         <v>171</v>
       </c>
       <c r="F15" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B15, C15, holiday!A$2:A$500)</f>
-        <v>121</v>
+        <f aca="false">NETWORKDAYS(B15, C15, holiday!A$2:A$499)</f>
+        <v>122</v>
       </c>
       <c r="G15" s="20" t="n">
         <f aca="false">D15/F15</f>
-        <v>0.495867768595041</v>
+        <v>0.491803278688525</v>
       </c>
       <c r="H15" s="21" t="n">
         <f aca="false">_xlfn.FLOOR.MATH(G15, 0.25)</f>
@@ -3713,7 +3713,7 @@
         <v>10</v>
       </c>
       <c r="F16" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B16, C16, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B16, C16, holiday!A$2:A$499)</f>
         <v>6</v>
       </c>
       <c r="G16" s="20" t="n">
@@ -3759,12 +3759,12 @@
         <v>171</v>
       </c>
       <c r="F17" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B17, C17, holiday!A$2:A$500)</f>
-        <v>121</v>
+        <f aca="false">NETWORKDAYS(B17, C17, holiday!A$2:A$499)</f>
+        <v>122</v>
       </c>
       <c r="G17" s="20" t="n">
         <f aca="false">D17/F17</f>
-        <v>0.826446280991736</v>
+        <v>0.819672131147541</v>
       </c>
       <c r="H17" s="21" t="n">
         <f aca="false">_xlfn.FLOOR.MATH(G17, 0.25)</f>
@@ -3805,7 +3805,7 @@
         <v>10</v>
       </c>
       <c r="F18" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B18, C18, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B18, C18, holiday!A$2:A$499)</f>
         <v>6</v>
       </c>
       <c r="G18" s="20" t="n">
@@ -3851,7 +3851,7 @@
         <v>26</v>
       </c>
       <c r="F19" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B19, C19, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B19, C19, holiday!A$2:A$499)</f>
         <v>19</v>
       </c>
       <c r="G19" s="20" t="n">
@@ -3897,7 +3897,7 @@
         <v>501</v>
       </c>
       <c r="F20" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B20, C20, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B20, C20, holiday!A$2:A$499)</f>
         <v>357</v>
       </c>
       <c r="G20" s="20" t="n">
@@ -3943,7 +3943,7 @@
         <v>56</v>
       </c>
       <c r="F21" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B21, C21, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B21, C21, holiday!A$2:A$499)</f>
         <v>40</v>
       </c>
       <c r="G21" s="20" t="n">
@@ -3989,12 +3989,12 @@
         <v>61</v>
       </c>
       <c r="F22" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B22, C22, holiday!A$2:A$500)</f>
-        <v>42</v>
+        <f aca="false">NETWORKDAYS(B22, C22, holiday!A$2:A$499)</f>
+        <v>43</v>
       </c>
       <c r="G22" s="20" t="n">
         <f aca="false">D22/F22</f>
-        <v>0.952380952380952</v>
+        <v>0.930232558139535</v>
       </c>
       <c r="H22" s="21" t="n">
         <f aca="false">_xlfn.FLOOR.MATH(G22, 0.25)</f>
@@ -4035,7 +4035,7 @@
         <v>8</v>
       </c>
       <c r="F23" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B23, C23, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B23, C23, holiday!A$2:A$499)</f>
         <v>6</v>
       </c>
       <c r="G23" s="20" t="n">
@@ -4081,7 +4081,7 @@
         <v>26</v>
       </c>
       <c r="F24" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B24, C24, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B24, C24, holiday!A$2:A$499)</f>
         <v>19</v>
       </c>
       <c r="G24" s="20" t="n">
@@ -4127,7 +4127,7 @@
         <v>151</v>
       </c>
       <c r="F25" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B25, C25, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B25, C25, holiday!A$2:A$499)</f>
         <v>108</v>
       </c>
       <c r="G25" s="20" t="n">
@@ -4173,7 +4173,7 @@
         <v>25</v>
       </c>
       <c r="F26" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B26, C26, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B26, C26, holiday!A$2:A$499)</f>
         <v>17</v>
       </c>
       <c r="G26" s="20" t="n">
@@ -4219,12 +4219,12 @@
         <v>91</v>
       </c>
       <c r="F27" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B27, C27, holiday!A$2:A$500)</f>
-        <v>64</v>
+        <f aca="false">NETWORKDAYS(B27, C27, holiday!A$2:A$499)</f>
+        <v>65</v>
       </c>
       <c r="G27" s="20" t="n">
         <f aca="false">D27/F27</f>
-        <v>0.703125</v>
+        <v>0.692307692307692</v>
       </c>
       <c r="H27" s="21" t="n">
         <f aca="false">_xlfn.FLOOR.MATH(G27, 0.25)</f>
@@ -4265,7 +4265,7 @@
         <v>31</v>
       </c>
       <c r="F28" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B28, C28, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B28, C28, holiday!A$2:A$499)</f>
         <v>22</v>
       </c>
       <c r="G28" s="20" t="n">
@@ -4311,12 +4311,12 @@
         <v>171</v>
       </c>
       <c r="F29" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B29, C29, holiday!A$2:A$500)</f>
-        <v>121</v>
+        <f aca="false">NETWORKDAYS(B29, C29, holiday!A$2:A$499)</f>
+        <v>122</v>
       </c>
       <c r="G29" s="20" t="n">
         <f aca="false">D29/F29</f>
-        <v>0.537190082644628</v>
+        <v>0.532786885245902</v>
       </c>
       <c r="H29" s="21" t="n">
         <f aca="false">_xlfn.FLOOR.MATH(G29, 0.25)</f>
@@ -4357,7 +4357,7 @@
         <v>46</v>
       </c>
       <c r="F30" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B30, C30, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B30, C30, holiday!A$2:A$499)</f>
         <v>32</v>
       </c>
       <c r="G30" s="20" t="n">
@@ -4403,12 +4403,12 @@
         <v>274</v>
       </c>
       <c r="F31" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B31, C31, holiday!A$2:A$500)</f>
-        <v>194</v>
+        <f aca="false">NETWORKDAYS(B31, C31, holiday!A$2:A$499)</f>
+        <v>195</v>
       </c>
       <c r="G31" s="20" t="n">
         <f aca="false">D31/F31</f>
-        <v>0.670103092783505</v>
+        <v>0.666666666666667</v>
       </c>
       <c r="H31" s="21" t="n">
         <f aca="false">_xlfn.FLOOR.MATH(G31, 0.25)</f>
@@ -4449,7 +4449,7 @@
         <v>31</v>
       </c>
       <c r="F32" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B32, C32, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B32, C32, holiday!A$2:A$499)</f>
         <v>22</v>
       </c>
       <c r="G32" s="20" t="n">
@@ -4495,7 +4495,7 @@
         <v>15</v>
       </c>
       <c r="F33" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B33, C33, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B33, C33, holiday!A$2:A$499)</f>
         <v>11</v>
       </c>
       <c r="G33" s="20" t="n">
@@ -4541,7 +4541,7 @@
         <v>174</v>
       </c>
       <c r="F34" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B34, C34, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B34, C34, holiday!A$2:A$499)</f>
         <v>124</v>
       </c>
       <c r="G34" s="20" t="n">
@@ -4587,7 +4587,7 @@
         <v>32</v>
       </c>
       <c r="F35" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B35, C35, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B35, C35, holiday!A$2:A$499)</f>
         <v>23</v>
       </c>
       <c r="G35" s="20" t="n">
@@ -4633,12 +4633,12 @@
         <v>56</v>
       </c>
       <c r="F36" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B36, C36, holiday!A$2:A$500)</f>
-        <v>39</v>
+        <f aca="false">NETWORKDAYS(B36, C36, holiday!A$2:A$499)</f>
+        <v>40</v>
       </c>
       <c r="G36" s="20" t="n">
         <f aca="false">D36/F36</f>
-        <v>0.641025641025641</v>
+        <v>0.625</v>
       </c>
       <c r="H36" s="21" t="n">
         <f aca="false">_xlfn.FLOOR.MATH(G36, 0.25)</f>
@@ -4679,7 +4679,7 @@
         <v>6</v>
       </c>
       <c r="F37" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B37, C37, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B37, C37, holiday!A$2:A$499)</f>
         <v>4</v>
       </c>
       <c r="G37" s="20" t="n">
@@ -4725,7 +4725,7 @@
         <v>6</v>
       </c>
       <c r="F38" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B38, C38, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B38, C38, holiday!A$2:A$499)</f>
         <v>4</v>
       </c>
       <c r="G38" s="20" t="n">
@@ -4771,7 +4771,7 @@
         <v>121</v>
       </c>
       <c r="F39" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B39, C39, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B39, C39, holiday!A$2:A$499)</f>
         <v>86</v>
       </c>
       <c r="G39" s="20" t="n">
@@ -4817,7 +4817,7 @@
         <v>16</v>
       </c>
       <c r="F40" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B40, C40, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B40, C40, holiday!A$2:A$499)</f>
         <v>10</v>
       </c>
       <c r="G40" s="20" t="n">
@@ -4863,7 +4863,7 @@
         <v>16</v>
       </c>
       <c r="F41" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B41, C41, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B41, C41, holiday!A$2:A$499)</f>
         <v>12</v>
       </c>
       <c r="G41" s="20" t="n">
@@ -4909,7 +4909,7 @@
         <v>271</v>
       </c>
       <c r="F42" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B42, C42, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B42, C42, holiday!A$2:A$499)</f>
         <v>193</v>
       </c>
       <c r="G42" s="20" t="n">
@@ -4955,7 +4955,7 @@
         <v>23</v>
       </c>
       <c r="F43" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B43, C43, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B43, C43, holiday!A$2:A$499)</f>
         <v>17</v>
       </c>
       <c r="G43" s="20" t="n">
@@ -5001,12 +5001,12 @@
         <v>74</v>
       </c>
       <c r="F44" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B44, C44, holiday!A$2:A$500)</f>
-        <v>52</v>
+        <f aca="false">NETWORKDAYS(B44, C44, holiday!A$2:A$499)</f>
+        <v>53</v>
       </c>
       <c r="G44" s="20" t="n">
         <f aca="false">D44/F44</f>
-        <v>0.384615384615385</v>
+        <v>0.377358490566038</v>
       </c>
       <c r="H44" s="21" t="n">
         <f aca="false">_xlfn.FLOOR.MATH(G44, 0.25)</f>
@@ -5047,7 +5047,7 @@
         <v>46</v>
       </c>
       <c r="F45" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B45, C45, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B45, C45, holiday!A$2:A$499)</f>
         <v>32</v>
       </c>
       <c r="G45" s="20" t="n">
@@ -5093,12 +5093,12 @@
         <v>91</v>
       </c>
       <c r="F46" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B46, C46, holiday!A$2:A$500)</f>
-        <v>64</v>
+        <f aca="false">NETWORKDAYS(B46, C46, holiday!A$2:A$499)</f>
+        <v>65</v>
       </c>
       <c r="G46" s="20" t="n">
         <f aca="false">D46/F46</f>
-        <v>0.3125</v>
+        <v>0.307692307692308</v>
       </c>
       <c r="H46" s="21" t="n">
         <f aca="false">_xlfn.FLOOR.MATH(G46, 0.25)</f>
@@ -5139,7 +5139,7 @@
         <v>31</v>
       </c>
       <c r="F47" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B47, C47, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B47, C47, holiday!A$2:A$499)</f>
         <v>22</v>
       </c>
       <c r="G47" s="20" t="n">
@@ -5185,12 +5185,12 @@
         <v>132</v>
       </c>
       <c r="F48" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B48, C48, holiday!A$2:A$500)</f>
-        <v>92</v>
+        <f aca="false">NETWORKDAYS(B48, C48, holiday!A$2:A$499)</f>
+        <v>93</v>
       </c>
       <c r="G48" s="20" t="n">
         <f aca="false">D48/F48</f>
-        <v>0.434782608695652</v>
+        <v>0.43010752688172</v>
       </c>
       <c r="H48" s="21" t="n">
         <f aca="false">_xlfn.FLOOR.MATH(G48, 0.25)</f>
@@ -5231,7 +5231,7 @@
         <v>46</v>
       </c>
       <c r="F49" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B49, C49, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B49, C49, holiday!A$2:A$499)</f>
         <v>34</v>
       </c>
       <c r="G49" s="20" t="n">
@@ -5277,12 +5277,12 @@
         <v>244</v>
       </c>
       <c r="F50" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B50, C50, holiday!A$2:A$500)</f>
-        <v>172</v>
+        <f aca="false">NETWORKDAYS(B50, C50, holiday!A$2:A$499)</f>
+        <v>173</v>
       </c>
       <c r="G50" s="20" t="n">
         <f aca="false">D50/F50</f>
-        <v>0.465116279069767</v>
+        <v>0.46242774566474</v>
       </c>
       <c r="H50" s="21" t="n">
         <f aca="false">_xlfn.FLOOR.MATH(G50, 0.25)</f>
@@ -5323,7 +5323,7 @@
         <v>46</v>
       </c>
       <c r="F51" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B51, C51, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B51, C51, holiday!A$2:A$499)</f>
         <v>34</v>
       </c>
       <c r="G51" s="20" t="n">
@@ -5369,7 +5369,7 @@
         <v>24</v>
       </c>
       <c r="F52" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B52, C52, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B52, C52, holiday!A$2:A$499)</f>
         <v>16</v>
       </c>
       <c r="G52" s="20" t="n">
@@ -5415,7 +5415,7 @@
         <v>130</v>
       </c>
       <c r="F53" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B53, C53, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B53, C53, holiday!A$2:A$499)</f>
         <v>93</v>
       </c>
       <c r="G53" s="20" t="n">
@@ -5461,7 +5461,7 @@
         <v>46</v>
       </c>
       <c r="F54" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B54, C54, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B54, C54, holiday!A$2:A$499)</f>
         <v>32</v>
       </c>
       <c r="G54" s="20" t="n">
@@ -5507,7 +5507,7 @@
         <v>30</v>
       </c>
       <c r="F55" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B55, C55, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B55, C55, holiday!A$2:A$499)</f>
         <v>21</v>
       </c>
       <c r="G55" s="20" t="n">
@@ -5553,7 +5553,7 @@
         <v>196</v>
       </c>
       <c r="F56" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B56, C56, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B56, C56, holiday!A$2:A$499)</f>
         <v>139</v>
       </c>
       <c r="G56" s="20" t="n">
@@ -5599,7 +5599,7 @@
         <v>29</v>
       </c>
       <c r="F57" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B57, C57, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B57, C57, holiday!A$2:A$499)</f>
         <v>20</v>
       </c>
       <c r="G57" s="20" t="n">
@@ -5645,7 +5645,7 @@
         <v>31</v>
       </c>
       <c r="F58" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B58, C58, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B58, C58, holiday!A$2:A$499)</f>
         <v>22</v>
       </c>
       <c r="G58" s="20" t="n">
@@ -5691,7 +5691,7 @@
         <v>131</v>
       </c>
       <c r="F59" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B59, C59, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B59, C59, holiday!A$2:A$499)</f>
         <v>93</v>
       </c>
       <c r="G59" s="20" t="n">
@@ -5737,7 +5737,7 @@
         <v>8</v>
       </c>
       <c r="F60" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B60, C60, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B60, C60, holiday!A$2:A$499)</f>
         <v>6</v>
       </c>
       <c r="G60" s="20" t="n">
@@ -5783,7 +5783,7 @@
         <v>6</v>
       </c>
       <c r="F61" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B61, C61, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B61, C61, holiday!A$2:A$499)</f>
         <v>5</v>
       </c>
       <c r="G61" s="20" t="n">
@@ -5829,7 +5829,7 @@
         <v>46</v>
       </c>
       <c r="F62" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B62, C62, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B62, C62, holiday!A$2:A$499)</f>
         <v>33</v>
       </c>
       <c r="G62" s="20" t="n">
@@ -5875,7 +5875,7 @@
         <v>13</v>
       </c>
       <c r="F63" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B63, C63, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B63, C63, holiday!A$2:A$499)</f>
         <v>9</v>
       </c>
       <c r="G63" s="20" t="n">
@@ -5921,7 +5921,7 @@
         <v>11</v>
       </c>
       <c r="F64" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B64, C64, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B64, C64, holiday!A$2:A$499)</f>
         <v>8</v>
       </c>
       <c r="G64" s="20" t="n">
@@ -5967,7 +5967,7 @@
         <v>181</v>
       </c>
       <c r="F65" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B65, C65, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B65, C65, holiday!A$2:A$499)</f>
         <v>128</v>
       </c>
       <c r="G65" s="20" t="n">
@@ -6013,7 +6013,7 @@
         <v>20</v>
       </c>
       <c r="F66" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B66, C66, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B66, C66, holiday!A$2:A$499)</f>
         <v>14</v>
       </c>
       <c r="G66" s="20" t="n">
@@ -6059,12 +6059,12 @@
         <v>81</v>
       </c>
       <c r="F67" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B67, C67, holiday!A$2:A$500)</f>
-        <v>57</v>
+        <f aca="false">NETWORKDAYS(B67, C67, holiday!A$2:A$499)</f>
+        <v>58</v>
       </c>
       <c r="G67" s="20" t="n">
         <f aca="false">D67/F67</f>
-        <v>0.87719298245614</v>
+        <v>0.862068965517241</v>
       </c>
       <c r="H67" s="21" t="n">
         <f aca="false">_xlfn.FLOOR.MATH(G67, 0.25)</f>
@@ -6105,7 +6105,7 @@
         <v>10</v>
       </c>
       <c r="F68" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B68, C68, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B68, C68, holiday!A$2:A$499)</f>
         <v>7</v>
       </c>
       <c r="G68" s="20" t="n">
@@ -6151,12 +6151,12 @@
         <v>171</v>
       </c>
       <c r="F69" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B69, C69, holiday!A$2:A$500)</f>
-        <v>121</v>
+        <f aca="false">NETWORKDAYS(B69, C69, holiday!A$2:A$499)</f>
+        <v>122</v>
       </c>
       <c r="G69" s="20" t="n">
         <f aca="false">D69/F69</f>
-        <v>0.247933884297521</v>
+        <v>0.245901639344262</v>
       </c>
       <c r="H69" s="21" t="n">
         <f aca="false">_xlfn.FLOOR.MATH(G69, 0.25)</f>
@@ -6197,7 +6197,7 @@
         <v>11</v>
       </c>
       <c r="F70" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B70, C70, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B70, C70, holiday!A$2:A$499)</f>
         <v>7</v>
       </c>
       <c r="G70" s="20" t="n">
@@ -6243,12 +6243,12 @@
         <v>21</v>
       </c>
       <c r="F71" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B71, C71, holiday!A$2:A$500)</f>
-        <v>14</v>
+        <f aca="false">NETWORKDAYS(B71, C71, holiday!A$2:A$499)</f>
+        <v>15</v>
       </c>
       <c r="G71" s="20" t="n">
         <f aca="false">D71/F71</f>
-        <v>1.42857142857143</v>
+        <v>1.33333333333333</v>
       </c>
       <c r="H71" s="21" t="n">
         <f aca="false">_xlfn.FLOOR.MATH(G71, 0.25)</f>
@@ -6289,7 +6289,7 @@
         <v>48</v>
       </c>
       <c r="F72" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B72, C72, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B72, C72, holiday!A$2:A$499)</f>
         <v>34</v>
       </c>
       <c r="G72" s="20" t="n">
@@ -6335,12 +6335,12 @@
         <v>81</v>
       </c>
       <c r="F73" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B73, C73, holiday!A$2:A$500)</f>
-        <v>57</v>
+        <f aca="false">NETWORKDAYS(B73, C73, holiday!A$2:A$499)</f>
+        <v>58</v>
       </c>
       <c r="G73" s="20" t="n">
         <f aca="false">D73/F73</f>
-        <v>0.175438596491228</v>
+        <v>0.172413793103448</v>
       </c>
       <c r="H73" s="21" t="n">
         <f aca="false">_xlfn.FLOOR.MATH(G73, 0.25)</f>
@@ -6381,7 +6381,7 @@
         <v>10</v>
       </c>
       <c r="F74" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B74, C74, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B74, C74, holiday!A$2:A$499)</f>
         <v>7</v>
       </c>
       <c r="G74" s="20" t="n">
@@ -6427,12 +6427,12 @@
         <v>21</v>
       </c>
       <c r="F75" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B75, C75, holiday!A$2:A$500)</f>
-        <v>14</v>
+        <f aca="false">NETWORKDAYS(B75, C75, holiday!A$2:A$499)</f>
+        <v>15</v>
       </c>
       <c r="G75" s="20" t="n">
         <f aca="false">D75/F75</f>
-        <v>1.07142857142857</v>
+        <v>1</v>
       </c>
       <c r="H75" s="21" t="n">
         <f aca="false">_xlfn.FLOOR.MATH(G75, 0.25)</f>
@@ -6473,7 +6473,7 @@
         <v>13</v>
       </c>
       <c r="F76" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B76, C76, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B76, C76, holiday!A$2:A$499)</f>
         <v>9</v>
       </c>
       <c r="G76" s="20" t="n">
@@ -6519,12 +6519,12 @@
         <v>81</v>
       </c>
       <c r="F77" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B77, C77, holiday!A$2:A$500)</f>
-        <v>57</v>
+        <f aca="false">NETWORKDAYS(B77, C77, holiday!A$2:A$499)</f>
+        <v>58</v>
       </c>
       <c r="G77" s="20" t="n">
         <f aca="false">D77/F77</f>
-        <v>0.701754385964912</v>
+        <v>0.689655172413793</v>
       </c>
       <c r="H77" s="21" t="n">
         <f aca="false">_xlfn.FLOOR.MATH(G77, 0.25)</f>
@@ -6565,7 +6565,7 @@
         <v>9</v>
       </c>
       <c r="F78" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B78, C78, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B78, C78, holiday!A$2:A$499)</f>
         <v>6</v>
       </c>
       <c r="G78" s="20" t="n">
@@ -6611,12 +6611,12 @@
         <v>46</v>
       </c>
       <c r="F79" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B79, C79, holiday!A$2:A$500)</f>
-        <v>32</v>
+        <f aca="false">NETWORKDAYS(B79, C79, holiday!A$2:A$499)</f>
+        <v>33</v>
       </c>
       <c r="G79" s="20" t="n">
         <f aca="false">D79/F79</f>
-        <v>0.3125</v>
+        <v>0.303030303030303</v>
       </c>
       <c r="H79" s="21" t="n">
         <f aca="false">_xlfn.FLOOR.MATH(G79, 0.25)</f>
@@ -6657,7 +6657,7 @@
         <v>10</v>
       </c>
       <c r="F80" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B80, C80, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B80, C80, holiday!A$2:A$499)</f>
         <v>7</v>
       </c>
       <c r="G80" s="20" t="n">
@@ -6703,7 +6703,7 @@
         <v>16</v>
       </c>
       <c r="F81" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B81, C81, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B81, C81, holiday!A$2:A$499)</f>
         <v>10</v>
       </c>
       <c r="G81" s="20" t="n">
@@ -6749,7 +6749,7 @@
         <v>211</v>
       </c>
       <c r="F82" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B82, C82, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B82, C82, holiday!A$2:A$499)</f>
         <v>150</v>
       </c>
       <c r="G82" s="20" t="n">
@@ -6795,7 +6795,7 @@
         <v>16</v>
       </c>
       <c r="F83" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B83, C83, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B83, C83, holiday!A$2:A$499)</f>
         <v>12</v>
       </c>
       <c r="G83" s="20" t="n">
@@ -6841,7 +6841,7 @@
         <v>16</v>
       </c>
       <c r="F84" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B84, C84, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B84, C84, holiday!A$2:A$499)</f>
         <v>11</v>
       </c>
       <c r="G84" s="20" t="n">
@@ -6887,7 +6887,7 @@
         <v>271</v>
       </c>
       <c r="F85" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B85, C85, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B85, C85, holiday!A$2:A$499)</f>
         <v>193</v>
       </c>
       <c r="G85" s="20" t="n">
@@ -6933,7 +6933,7 @@
         <v>19</v>
       </c>
       <c r="F86" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B86, C86, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B86, C86, holiday!A$2:A$499)</f>
         <v>13</v>
       </c>
       <c r="G86" s="20" t="n">
@@ -6979,20 +6979,20 @@
         <v>76</v>
       </c>
       <c r="F87" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B87, C87, holiday!A$2:A$500)</f>
-        <v>53</v>
+        <f aca="false">NETWORKDAYS(B87, C87, holiday!A$2:A$499)</f>
+        <v>54</v>
       </c>
       <c r="G87" s="20" t="n">
         <f aca="false">D87/F87</f>
-        <v>0.754716981132076</v>
+        <v>0.740740740740741</v>
       </c>
       <c r="H87" s="21" t="n">
         <f aca="false">_xlfn.FLOOR.MATH(G87, 0.25)</f>
-        <v>0.75</v>
+        <v>0.5</v>
       </c>
       <c r="I87" s="21" t="n">
         <f aca="false">H87 + 0.25</f>
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="J87" s="2" t="b">
         <f aca="false">COUNTIF(assign!$B$1:$B$563, A87) &gt; 0</f>
@@ -7025,7 +7025,7 @@
         <v>8</v>
       </c>
       <c r="F88" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B88, C88, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B88, C88, holiday!A$2:A$499)</f>
         <v>6</v>
       </c>
       <c r="G88" s="20" t="n">
@@ -7071,12 +7071,12 @@
         <v>56</v>
       </c>
       <c r="F89" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B89, C89, holiday!A$2:A$500)</f>
-        <v>39</v>
+        <f aca="false">NETWORKDAYS(B89, C89, holiday!A$2:A$499)</f>
+        <v>40</v>
       </c>
       <c r="G89" s="20" t="n">
         <f aca="false">D89/F89</f>
-        <v>0.769230769230769</v>
+        <v>0.75</v>
       </c>
       <c r="H89" s="21" t="n">
         <f aca="false">_xlfn.FLOOR.MATH(G89, 0.25)</f>
@@ -7117,7 +7117,7 @@
         <v>6</v>
       </c>
       <c r="F90" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B90, C90, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B90, C90, holiday!A$2:A$499)</f>
         <v>4</v>
       </c>
       <c r="G90" s="20" t="n">
@@ -7163,12 +7163,12 @@
         <v>86</v>
       </c>
       <c r="F91" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B91, C91, holiday!A$2:A$500)</f>
-        <v>61</v>
+        <f aca="false">NETWORKDAYS(B91, C91, holiday!A$2:A$499)</f>
+        <v>62</v>
       </c>
       <c r="G91" s="20" t="n">
         <f aca="false">D91/F91</f>
-        <v>0.983606557377049</v>
+        <v>0.967741935483871</v>
       </c>
       <c r="H91" s="21" t="n">
         <f aca="false">_xlfn.FLOOR.MATH(G91, 0.25)</f>
@@ -7209,7 +7209,7 @@
         <v>11</v>
       </c>
       <c r="F92" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B92, C92, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B92, C92, holiday!A$2:A$499)</f>
         <v>7</v>
       </c>
       <c r="G92" s="20" t="n">
@@ -7255,12 +7255,12 @@
         <v>141</v>
       </c>
       <c r="F93" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B93, C93, holiday!A$2:A$500)</f>
-        <v>99</v>
+        <f aca="false">NETWORKDAYS(B93, C93, holiday!A$2:A$499)</f>
+        <v>100</v>
       </c>
       <c r="G93" s="20" t="n">
         <f aca="false">D93/F93</f>
-        <v>0.303030303030303</v>
+        <v>0.3</v>
       </c>
       <c r="H93" s="21" t="n">
         <f aca="false">_xlfn.FLOOR.MATH(G93, 0.25)</f>
@@ -7301,7 +7301,7 @@
         <v>12</v>
       </c>
       <c r="F94" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B94, C94, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B94, C94, holiday!A$2:A$499)</f>
         <v>8</v>
       </c>
       <c r="G94" s="20" t="n">
@@ -7347,7 +7347,7 @@
         <v>26</v>
       </c>
       <c r="F95" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B95, C95, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B95, C95, holiday!A$2:A$499)</f>
         <v>18</v>
       </c>
       <c r="G95" s="20" t="n">
@@ -7393,7 +7393,7 @@
         <v>131</v>
       </c>
       <c r="F96" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B96, C96, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B96, C96, holiday!A$2:A$499)</f>
         <v>92</v>
       </c>
       <c r="G96" s="20" t="n">
@@ -7439,7 +7439,7 @@
         <v>14</v>
       </c>
       <c r="F97" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B97, C97, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B97, C97, holiday!A$2:A$499)</f>
         <v>10</v>
       </c>
       <c r="G97" s="20" t="n">
@@ -7485,12 +7485,12 @@
         <v>81</v>
       </c>
       <c r="F98" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B98, C98, holiday!A$2:A$500)</f>
-        <v>57</v>
+        <f aca="false">NETWORKDAYS(B98, C98, holiday!A$2:A$499)</f>
+        <v>58</v>
       </c>
       <c r="G98" s="20" t="n">
         <f aca="false">D98/F98</f>
-        <v>0.350877192982456</v>
+        <v>0.344827586206897</v>
       </c>
       <c r="H98" s="21" t="n">
         <f aca="false">_xlfn.FLOOR.MATH(G98, 0.25)</f>
@@ -7531,7 +7531,7 @@
         <v>9</v>
       </c>
       <c r="F99" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B99, C99, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B99, C99, holiday!A$2:A$499)</f>
         <v>6</v>
       </c>
       <c r="G99" s="20" t="n">
@@ -7577,7 +7577,7 @@
         <v>16</v>
       </c>
       <c r="F100" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B100, C100, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B100, C100, holiday!A$2:A$499)</f>
         <v>10</v>
       </c>
       <c r="G100" s="20" t="n">
@@ -7623,7 +7623,7 @@
         <v>211</v>
       </c>
       <c r="F101" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B101, C101, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B101, C101, holiday!A$2:A$499)</f>
         <v>150</v>
       </c>
       <c r="G101" s="20" t="n">
@@ -7669,7 +7669,7 @@
         <v>16</v>
       </c>
       <c r="F102" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B102, C102, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B102, C102, holiday!A$2:A$499)</f>
         <v>12</v>
       </c>
       <c r="G102" s="20" t="n">
@@ -7715,7 +7715,7 @@
         <v>16</v>
       </c>
       <c r="F103" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B103, C103, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B103, C103, holiday!A$2:A$499)</f>
         <v>10</v>
       </c>
       <c r="G103" s="20" t="n">
@@ -7761,7 +7761,7 @@
         <v>171</v>
       </c>
       <c r="F104" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B104, C104, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B104, C104, holiday!A$2:A$499)</f>
         <v>122</v>
       </c>
       <c r="G104" s="20" t="n">
@@ -7807,7 +7807,7 @@
         <v>12</v>
       </c>
       <c r="F105" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B105, C105, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B105, C105, holiday!A$2:A$499)</f>
         <v>8</v>
       </c>
       <c r="G105" s="20" t="n">
@@ -7853,12 +7853,12 @@
         <v>91</v>
       </c>
       <c r="F106" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B106, C106, holiday!A$2:A$500)</f>
-        <v>64</v>
+        <f aca="false">NETWORKDAYS(B106, C106, holiday!A$2:A$499)</f>
+        <v>65</v>
       </c>
       <c r="G106" s="20" t="n">
         <f aca="false">D106/F106</f>
-        <v>0.15625</v>
+        <v>0.153846153846154</v>
       </c>
       <c r="H106" s="21" t="n">
         <f aca="false">_xlfn.FLOOR.MATH(G106, 0.25)</f>
@@ -7899,7 +7899,7 @@
         <v>31</v>
       </c>
       <c r="F107" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B107, C107, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B107, C107, holiday!A$2:A$499)</f>
         <v>22</v>
       </c>
       <c r="G107" s="20" t="n">
@@ -7945,12 +7945,12 @@
         <v>171</v>
       </c>
       <c r="F108" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B108, C108, holiday!A$2:A$500)</f>
-        <v>121</v>
+        <f aca="false">NETWORKDAYS(B108, C108, holiday!A$2:A$499)</f>
+        <v>122</v>
       </c>
       <c r="G108" s="20" t="n">
         <f aca="false">D108/F108</f>
-        <v>0.0826446280991736</v>
+        <v>0.0819672131147541</v>
       </c>
       <c r="H108" s="21" t="n">
         <f aca="false">_xlfn.FLOOR.MATH(G108, 0.25)</f>
@@ -7991,7 +7991,7 @@
         <v>46</v>
       </c>
       <c r="F109" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B109, C109, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B109, C109, holiday!A$2:A$499)</f>
         <v>32</v>
       </c>
       <c r="G109" s="20" t="n">
@@ -8037,12 +8037,12 @@
         <v>156</v>
       </c>
       <c r="F110" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B110, C110, holiday!A$2:A$500)</f>
-        <v>110</v>
+        <f aca="false">NETWORKDAYS(B110, C110, holiday!A$2:A$499)</f>
+        <v>111</v>
       </c>
       <c r="G110" s="20" t="n">
         <f aca="false">D110/F110</f>
-        <v>0.136363636363636</v>
+        <v>0.135135135135135</v>
       </c>
       <c r="H110" s="21" t="n">
         <f aca="false">_xlfn.FLOOR.MATH(G110, 0.25)</f>
@@ -8083,7 +8083,7 @@
         <v>31</v>
       </c>
       <c r="F111" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B111, C111, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B111, C111, holiday!A$2:A$499)</f>
         <v>21</v>
       </c>
       <c r="G111" s="20" t="n">
@@ -8129,12 +8129,12 @@
         <v>56</v>
       </c>
       <c r="F112" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B112, C112, holiday!A$2:A$500)</f>
-        <v>39</v>
+        <f aca="false">NETWORKDAYS(B112, C112, holiday!A$2:A$499)</f>
+        <v>40</v>
       </c>
       <c r="G112" s="20" t="n">
         <f aca="false">D112/F112</f>
-        <v>0.128205128205128</v>
+        <v>0.125</v>
       </c>
       <c r="H112" s="21" t="n">
         <f aca="false">_xlfn.FLOOR.MATH(G112, 0.25)</f>
@@ -8175,7 +8175,7 @@
         <v>46</v>
       </c>
       <c r="F113" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B113, C113, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B113, C113, holiday!A$2:A$499)</f>
         <v>33</v>
       </c>
       <c r="G113" s="20" t="n">
@@ -8221,12 +8221,12 @@
         <v>74</v>
       </c>
       <c r="F114" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B114, C114, holiday!A$2:A$500)</f>
-        <v>52</v>
+        <f aca="false">NETWORKDAYS(B114, C114, holiday!A$2:A$499)</f>
+        <v>53</v>
       </c>
       <c r="G114" s="20" t="n">
         <f aca="false">D114/F114</f>
-        <v>0.0961538461538462</v>
+        <v>0.0943396226415094</v>
       </c>
       <c r="H114" s="21" t="n">
         <f aca="false">_xlfn.FLOOR.MATH(G114, 0.25)</f>
@@ -8267,7 +8267,7 @@
         <v>46</v>
       </c>
       <c r="F115" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B115, C115, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B115, C115, holiday!A$2:A$499)</f>
         <v>32</v>
       </c>
       <c r="G115" s="20" t="n">
@@ -8313,12 +8313,12 @@
         <v>132</v>
       </c>
       <c r="F116" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B116, C116, holiday!A$2:A$500)</f>
-        <v>92</v>
+        <f aca="false">NETWORKDAYS(B116, C116, holiday!A$2:A$499)</f>
+        <v>93</v>
       </c>
       <c r="G116" s="20" t="n">
         <f aca="false">D116/F116</f>
-        <v>0.108695652173913</v>
+        <v>0.10752688172043</v>
       </c>
       <c r="H116" s="21" t="n">
         <f aca="false">_xlfn.FLOOR.MATH(G116, 0.25)</f>
@@ -8359,7 +8359,7 @@
         <v>46</v>
       </c>
       <c r="F117" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B117, C117, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B117, C117, holiday!A$2:A$499)</f>
         <v>34</v>
       </c>
       <c r="G117" s="20" t="n">
@@ -8405,7 +8405,7 @@
         <v>24</v>
       </c>
       <c r="F118" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B118, C118, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B118, C118, holiday!A$2:A$499)</f>
         <v>16</v>
       </c>
       <c r="G118" s="20" t="n">
@@ -8451,7 +8451,7 @@
         <v>130</v>
       </c>
       <c r="F119" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B119, C119, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B119, C119, holiday!A$2:A$499)</f>
         <v>93</v>
       </c>
       <c r="G119" s="20" t="n">
@@ -8497,7 +8497,7 @@
         <v>46</v>
       </c>
       <c r="F120" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B120, C120, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B120, C120, holiday!A$2:A$499)</f>
         <v>32</v>
       </c>
       <c r="G120" s="20" t="n">
@@ -8543,7 +8543,7 @@
         <v>30</v>
       </c>
       <c r="F121" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B121, C121, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B121, C121, holiday!A$2:A$499)</f>
         <v>21</v>
       </c>
       <c r="G121" s="20" t="n">
@@ -8589,7 +8589,7 @@
         <v>196</v>
       </c>
       <c r="F122" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B122, C122, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B122, C122, holiday!A$2:A$499)</f>
         <v>139</v>
       </c>
       <c r="G122" s="20" t="n">
@@ -8635,7 +8635,7 @@
         <v>29</v>
       </c>
       <c r="F123" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B123, C123, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B123, C123, holiday!A$2:A$499)</f>
         <v>20</v>
       </c>
       <c r="G123" s="20" t="n">
@@ -8681,7 +8681,7 @@
         <v>30</v>
       </c>
       <c r="F124" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B124, C124, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B124, C124, holiday!A$2:A$499)</f>
         <v>21</v>
       </c>
       <c r="G124" s="20" t="n">
@@ -8727,7 +8727,7 @@
         <v>196</v>
       </c>
       <c r="F125" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B125, C125, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B125, C125, holiday!A$2:A$499)</f>
         <v>139</v>
       </c>
       <c r="G125" s="20" t="n">
@@ -8773,7 +8773,7 @@
         <v>29</v>
       </c>
       <c r="F126" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B126, C126, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B126, C126, holiday!A$2:A$499)</f>
         <v>20</v>
       </c>
       <c r="G126" s="20" t="n">
@@ -8819,12 +8819,12 @@
         <v>91</v>
       </c>
       <c r="F127" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B127, C127, holiday!A$2:A$500)</f>
-        <v>64</v>
+        <f aca="false">NETWORKDAYS(B127, C127, holiday!A$2:A$499)</f>
+        <v>65</v>
       </c>
       <c r="G127" s="20" t="n">
         <f aca="false">D127/F127</f>
-        <v>0.125</v>
+        <v>0.123076923076923</v>
       </c>
       <c r="H127" s="21" t="n">
         <f aca="false">_xlfn.FLOOR.MATH(G127, 0.25)</f>
@@ -8865,7 +8865,7 @@
         <v>31</v>
       </c>
       <c r="F128" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B128, C128, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B128, C128, holiday!A$2:A$499)</f>
         <v>22</v>
       </c>
       <c r="G128" s="20" t="n">
@@ -8911,12 +8911,12 @@
         <v>244</v>
       </c>
       <c r="F129" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B129, C129, holiday!A$2:A$500)</f>
-        <v>172</v>
+        <f aca="false">NETWORKDAYS(B129, C129, holiday!A$2:A$499)</f>
+        <v>173</v>
       </c>
       <c r="G129" s="20" t="n">
         <f aca="false">D129/F129</f>
-        <v>0.0872093023255814</v>
+        <v>0.0867052023121387</v>
       </c>
       <c r="H129" s="21" t="n">
         <f aca="false">_xlfn.FLOOR.MATH(G129, 0.25)</f>
@@ -8957,7 +8957,7 @@
         <v>46</v>
       </c>
       <c r="F130" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B130, C130, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B130, C130, holiday!A$2:A$499)</f>
         <v>34</v>
       </c>
       <c r="G130" s="20" t="n">
@@ -9003,12 +9003,12 @@
         <v>274</v>
       </c>
       <c r="F131" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B131, C131, holiday!A$2:A$500)</f>
-        <v>194</v>
+        <f aca="false">NETWORKDAYS(B131, C131, holiday!A$2:A$499)</f>
+        <v>195</v>
       </c>
       <c r="G131" s="20" t="n">
         <f aca="false">D131/F131</f>
-        <v>0.154639175257732</v>
+        <v>0.153846153846154</v>
       </c>
       <c r="H131" s="21" t="n">
         <f aca="false">_xlfn.FLOOR.MATH(G131, 0.25)</f>
@@ -9049,7 +9049,7 @@
         <v>31</v>
       </c>
       <c r="F132" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B132, C132, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B132, C132, holiday!A$2:A$499)</f>
         <v>22</v>
       </c>
       <c r="G132" s="20" t="n">
@@ -9095,7 +9095,7 @@
         <v>18</v>
       </c>
       <c r="F133" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B133, C133, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B133, C133, holiday!A$2:A$499)</f>
         <v>14</v>
       </c>
       <c r="G133" s="20" t="n">
@@ -9141,7 +9141,7 @@
         <v>123</v>
       </c>
       <c r="F134" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B134, C134, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B134, C134, holiday!A$2:A$499)</f>
         <v>86</v>
       </c>
       <c r="G134" s="20" t="n">
@@ -9187,7 +9187,7 @@
         <v>46</v>
       </c>
       <c r="F135" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B135, C135, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B135, C135, holiday!A$2:A$499)</f>
         <v>34</v>
       </c>
       <c r="G135" s="20" t="n">
@@ -9233,7 +9233,7 @@
         <v>20</v>
       </c>
       <c r="F136" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B136, C136, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B136, C136, holiday!A$2:A$499)</f>
         <v>15</v>
       </c>
       <c r="G136" s="20" t="n">
@@ -9279,7 +9279,7 @@
         <v>199</v>
       </c>
       <c r="F137" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B137, C137, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B137, C137, holiday!A$2:A$499)</f>
         <v>142</v>
       </c>
       <c r="G137" s="20" t="n">
@@ -9325,7 +9325,7 @@
         <v>32</v>
       </c>
       <c r="F138" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B138, C138, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B138, C138, holiday!A$2:A$499)</f>
         <v>23</v>
       </c>
       <c r="G138" s="20" t="n">
@@ -9371,7 +9371,7 @@
         <v>15</v>
       </c>
       <c r="F139" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B139, C139, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B139, C139, holiday!A$2:A$499)</f>
         <v>11</v>
       </c>
       <c r="G139" s="20" t="n">
@@ -9417,7 +9417,7 @@
         <v>174</v>
       </c>
       <c r="F140" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B140, C140, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B140, C140, holiday!A$2:A$499)</f>
         <v>124</v>
       </c>
       <c r="G140" s="20" t="n">
@@ -9463,7 +9463,7 @@
         <v>32</v>
       </c>
       <c r="F141" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B141, C141, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B141, C141, holiday!A$2:A$499)</f>
         <v>23</v>
       </c>
       <c r="G141" s="20" t="n">
@@ -9509,7 +9509,7 @@
         <v>6</v>
       </c>
       <c r="F142" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B142, C142, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B142, C142, holiday!A$2:A$499)</f>
         <v>5</v>
       </c>
       <c r="G142" s="20" t="n">
@@ -9555,7 +9555,7 @@
         <v>46</v>
       </c>
       <c r="F143" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B143, C143, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B143, C143, holiday!A$2:A$499)</f>
         <v>33</v>
       </c>
       <c r="G143" s="20" t="n">
@@ -9601,7 +9601,7 @@
         <v>13</v>
       </c>
       <c r="F144" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B144, C144, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B144, C144, holiday!A$2:A$499)</f>
         <v>9</v>
       </c>
       <c r="G144" s="20" t="n">
@@ -9647,7 +9647,7 @@
         <v>11</v>
       </c>
       <c r="F145" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B145, C145, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B145, C145, holiday!A$2:A$499)</f>
         <v>8</v>
       </c>
       <c r="G145" s="20" t="n">
@@ -9693,7 +9693,7 @@
         <v>181</v>
       </c>
       <c r="F146" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B146, C146, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B146, C146, holiday!A$2:A$499)</f>
         <v>128</v>
       </c>
       <c r="G146" s="20" t="n">
@@ -9739,7 +9739,7 @@
         <v>20</v>
       </c>
       <c r="F147" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B147, C147, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B147, C147, holiday!A$2:A$499)</f>
         <v>14</v>
       </c>
       <c r="G147" s="20" t="n">
@@ -9785,12 +9785,12 @@
         <v>21</v>
       </c>
       <c r="F148" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B148, C148, holiday!A$2:A$500)</f>
-        <v>14</v>
+        <f aca="false">NETWORKDAYS(B148, C148, holiday!A$2:A$499)</f>
+        <v>15</v>
       </c>
       <c r="G148" s="20" t="n">
         <f aca="false">D148/F148</f>
-        <v>1.07142857142857</v>
+        <v>1</v>
       </c>
       <c r="H148" s="21" t="n">
         <f aca="false">_xlfn.FLOOR.MATH(G148, 0.25)</f>
@@ -9831,7 +9831,7 @@
         <v>13</v>
       </c>
       <c r="F149" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B149, C149, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B149, C149, holiday!A$2:A$499)</f>
         <v>9</v>
       </c>
       <c r="G149" s="20" t="n">
@@ -9877,7 +9877,7 @@
         <v>26</v>
       </c>
       <c r="F150" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B150, C150, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B150, C150, holiday!A$2:A$499)</f>
         <v>19</v>
       </c>
       <c r="G150" s="20" t="n">
@@ -9923,7 +9923,7 @@
         <v>501</v>
       </c>
       <c r="F151" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B151, C151, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B151, C151, holiday!A$2:A$499)</f>
         <v>357</v>
       </c>
       <c r="G151" s="20" t="n">
@@ -9969,7 +9969,7 @@
         <v>56</v>
       </c>
       <c r="F152" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B152, C152, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B152, C152, holiday!A$2:A$499)</f>
         <v>40</v>
       </c>
       <c r="G152" s="20" t="n">
@@ -10015,7 +10015,7 @@
         <v>16</v>
       </c>
       <c r="F153" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B153, C153, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B153, C153, holiday!A$2:A$499)</f>
         <v>11</v>
       </c>
       <c r="G153" s="20" t="n">
@@ -10061,7 +10061,7 @@
         <v>271</v>
       </c>
       <c r="F154" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B154, C154, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B154, C154, holiday!A$2:A$499)</f>
         <v>193</v>
       </c>
       <c r="G154" s="20" t="n">
@@ -10107,7 +10107,7 @@
         <v>19</v>
       </c>
       <c r="F155" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B155, C155, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B155, C155, holiday!A$2:A$499)</f>
         <v>13</v>
       </c>
       <c r="G155" s="20" t="n">
@@ -10153,7 +10153,7 @@
         <v>26</v>
       </c>
       <c r="F156" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B156, C156, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B156, C156, holiday!A$2:A$499)</f>
         <v>19</v>
       </c>
       <c r="G156" s="20" t="n">
@@ -10199,7 +10199,7 @@
         <v>151</v>
       </c>
       <c r="F157" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B157, C157, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B157, C157, holiday!A$2:A$499)</f>
         <v>108</v>
       </c>
       <c r="G157" s="20" t="n">
@@ -10245,7 +10245,7 @@
         <v>25</v>
       </c>
       <c r="F158" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B158, C158, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B158, C158, holiday!A$2:A$499)</f>
         <v>17</v>
       </c>
       <c r="G158" s="20" t="n">
@@ -10291,12 +10291,12 @@
         <v>76</v>
       </c>
       <c r="F159" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B159, C159, holiday!A$2:A$500)</f>
-        <v>53</v>
+        <f aca="false">NETWORKDAYS(B159, C159, holiday!A$2:A$499)</f>
+        <v>54</v>
       </c>
       <c r="G159" s="20" t="n">
         <f aca="false">D159/F159</f>
-        <v>0.188679245283019</v>
+        <v>0.185185185185185</v>
       </c>
       <c r="H159" s="21" t="n">
         <f aca="false">_xlfn.FLOOR.MATH(G159, 0.25)</f>
@@ -10337,7 +10337,7 @@
         <v>8</v>
       </c>
       <c r="F160" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B160, C160, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B160, C160, holiday!A$2:A$499)</f>
         <v>6</v>
       </c>
       <c r="G160" s="20" t="n">
@@ -10383,12 +10383,12 @@
         <v>81</v>
       </c>
       <c r="F161" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B161, C161, holiday!A$2:A$500)</f>
-        <v>57</v>
+        <f aca="false">NETWORKDAYS(B161, C161, holiday!A$2:A$499)</f>
+        <v>58</v>
       </c>
       <c r="G161" s="20" t="n">
         <f aca="false">D161/F161</f>
-        <v>0.350877192982456</v>
+        <v>0.344827586206897</v>
       </c>
       <c r="H161" s="21" t="n">
         <f aca="false">_xlfn.FLOOR.MATH(G161, 0.25)</f>
@@ -10429,7 +10429,7 @@
         <v>10</v>
       </c>
       <c r="F162" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B162, C162, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B162, C162, holiday!A$2:A$499)</f>
         <v>7</v>
       </c>
       <c r="G162" s="20" t="n">
@@ -10475,12 +10475,12 @@
         <v>56</v>
       </c>
       <c r="F163" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B163, C163, holiday!A$2:A$500)</f>
-        <v>39</v>
+        <f aca="false">NETWORKDAYS(B163, C163, holiday!A$2:A$499)</f>
+        <v>40</v>
       </c>
       <c r="G163" s="20" t="n">
         <f aca="false">D163/F163</f>
-        <v>0.256410256410256</v>
+        <v>0.25</v>
       </c>
       <c r="H163" s="21" t="n">
         <f aca="false">_xlfn.FLOOR.MATH(G163, 0.25)</f>
@@ -10521,7 +10521,7 @@
         <v>6</v>
       </c>
       <c r="F164" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B164, C164, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B164, C164, holiday!A$2:A$499)</f>
         <v>4</v>
       </c>
       <c r="G164" s="20" t="n">
@@ -10567,12 +10567,12 @@
         <v>56</v>
       </c>
       <c r="F165" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B165, C165, holiday!A$2:A$500)</f>
-        <v>39</v>
+        <f aca="false">NETWORKDAYS(B165, C165, holiday!A$2:A$499)</f>
+        <v>40</v>
       </c>
       <c r="G165" s="20" t="n">
         <f aca="false">D165/F165</f>
-        <v>0.384615384615385</v>
+        <v>0.375</v>
       </c>
       <c r="H165" s="21" t="n">
         <f aca="false">_xlfn.FLOOR.MATH(G165, 0.25)</f>
@@ -10613,7 +10613,7 @@
         <v>6</v>
       </c>
       <c r="F166" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B166, C166, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B166, C166, holiday!A$2:A$499)</f>
         <v>4</v>
       </c>
       <c r="G166" s="20" t="n">
@@ -10659,12 +10659,12 @@
         <v>86</v>
       </c>
       <c r="F167" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B167, C167, holiday!A$2:A$500)</f>
-        <v>61</v>
+        <f aca="false">NETWORKDAYS(B167, C167, holiday!A$2:A$499)</f>
+        <v>62</v>
       </c>
       <c r="G167" s="20" t="n">
         <f aca="false">D167/F167</f>
-        <v>0.491803278688525</v>
+        <v>0.483870967741936</v>
       </c>
       <c r="H167" s="21" t="n">
         <f aca="false">_xlfn.FLOOR.MATH(G167, 0.25)</f>
@@ -10705,7 +10705,7 @@
         <v>11</v>
       </c>
       <c r="F168" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B168, C168, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B168, C168, holiday!A$2:A$499)</f>
         <v>7</v>
       </c>
       <c r="G168" s="20" t="n">
@@ -10751,12 +10751,12 @@
         <v>171</v>
       </c>
       <c r="F169" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B169, C169, holiday!A$2:A$500)</f>
-        <v>121</v>
+        <f aca="false">NETWORKDAYS(B169, C169, holiday!A$2:A$499)</f>
+        <v>122</v>
       </c>
       <c r="G169" s="20" t="n">
         <f aca="false">D169/F169</f>
-        <v>0.247933884297521</v>
+        <v>0.245901639344262</v>
       </c>
       <c r="H169" s="21" t="n">
         <f aca="false">_xlfn.FLOOR.MATH(G169, 0.25)</f>
@@ -10797,7 +10797,7 @@
         <v>10</v>
       </c>
       <c r="F170" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B170, C170, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B170, C170, holiday!A$2:A$499)</f>
         <v>6</v>
       </c>
       <c r="G170" s="20" t="n">
@@ -10843,12 +10843,12 @@
         <v>171</v>
       </c>
       <c r="F171" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B171, C171, holiday!A$2:A$500)</f>
-        <v>121</v>
+        <f aca="false">NETWORKDAYS(B171, C171, holiday!A$2:A$499)</f>
+        <v>122</v>
       </c>
       <c r="G171" s="20" t="n">
         <f aca="false">D171/F171</f>
-        <v>0.330578512396694</v>
+        <v>0.327868852459016</v>
       </c>
       <c r="H171" s="21" t="n">
         <f aca="false">_xlfn.FLOOR.MATH(G171, 0.25)</f>
@@ -10889,7 +10889,7 @@
         <v>10</v>
       </c>
       <c r="F172" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B172, C172, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B172, C172, holiday!A$2:A$499)</f>
         <v>6</v>
       </c>
       <c r="G172" s="20" t="n">
@@ -10935,7 +10935,7 @@
         <v>31</v>
       </c>
       <c r="F173" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B173, C173, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B173, C173, holiday!A$2:A$499)</f>
         <v>22</v>
       </c>
       <c r="G173" s="20" t="n">
@@ -10981,7 +10981,7 @@
         <v>131</v>
       </c>
       <c r="F174" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B174, C174, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B174, C174, holiday!A$2:A$499)</f>
         <v>93</v>
       </c>
       <c r="G174" s="20" t="n">
@@ -11027,7 +11027,7 @@
         <v>8</v>
       </c>
       <c r="F175" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B175, C175, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B175, C175, holiday!A$2:A$499)</f>
         <v>6</v>
       </c>
       <c r="G175" s="20" t="n">
@@ -11073,12 +11073,12 @@
         <v>171</v>
       </c>
       <c r="F176" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B176, C176, holiday!A$2:A$500)</f>
-        <v>121</v>
+        <f aca="false">NETWORKDAYS(B176, C176, holiday!A$2:A$499)</f>
+        <v>122</v>
       </c>
       <c r="G176" s="20" t="n">
         <f aca="false">D176/F176</f>
-        <v>0.165289256198347</v>
+        <v>0.163934426229508</v>
       </c>
       <c r="H176" s="21" t="n">
         <f aca="false">_xlfn.FLOOR.MATH(G176, 0.25)</f>
@@ -11119,7 +11119,7 @@
         <v>11</v>
       </c>
       <c r="F177" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B177, C177, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B177, C177, holiday!A$2:A$499)</f>
         <v>7</v>
       </c>
       <c r="G177" s="20" t="n">
@@ -11165,12 +11165,12 @@
         <v>21</v>
       </c>
       <c r="F178" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B178, C178, holiday!A$2:A$500)</f>
-        <v>14</v>
+        <f aca="false">NETWORKDAYS(B178, C178, holiday!A$2:A$499)</f>
+        <v>15</v>
       </c>
       <c r="G178" s="20" t="n">
         <f aca="false">D178/F178</f>
-        <v>0.714285714285714</v>
+        <v>0.666666666666667</v>
       </c>
       <c r="H178" s="21" t="n">
         <f aca="false">_xlfn.FLOOR.MATH(G178, 0.25)</f>
@@ -11211,7 +11211,7 @@
         <v>48</v>
       </c>
       <c r="F179" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B179, C179, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B179, C179, holiday!A$2:A$499)</f>
         <v>34</v>
       </c>
       <c r="G179" s="20" t="n">
@@ -11257,12 +11257,12 @@
         <v>81</v>
       </c>
       <c r="F180" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B180, C180, holiday!A$2:A$500)</f>
-        <v>57</v>
+        <f aca="false">NETWORKDAYS(B180, C180, holiday!A$2:A$499)</f>
+        <v>58</v>
       </c>
       <c r="G180" s="20" t="n">
         <f aca="false">D180/F180</f>
-        <v>0.87719298245614</v>
+        <v>0.862068965517241</v>
       </c>
       <c r="H180" s="21" t="n">
         <f aca="false">_xlfn.FLOOR.MATH(G180, 0.25)</f>
@@ -11303,7 +11303,7 @@
         <v>10</v>
       </c>
       <c r="F181" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B181, C181, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B181, C181, holiday!A$2:A$499)</f>
         <v>7</v>
       </c>
       <c r="G181" s="20" t="n">
@@ -11349,12 +11349,12 @@
         <v>46</v>
       </c>
       <c r="F182" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B182, C182, holiday!A$2:A$500)</f>
-        <v>32</v>
+        <f aca="false">NETWORKDAYS(B182, C182, holiday!A$2:A$499)</f>
+        <v>33</v>
       </c>
       <c r="G182" s="20" t="n">
         <f aca="false">D182/F182</f>
-        <v>0.3125</v>
+        <v>0.303030303030303</v>
       </c>
       <c r="H182" s="21" t="n">
         <f aca="false">_xlfn.FLOOR.MATH(G182, 0.25)</f>
@@ -11395,7 +11395,7 @@
         <v>10</v>
       </c>
       <c r="F183" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B183, C183, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B183, C183, holiday!A$2:A$499)</f>
         <v>7</v>
       </c>
       <c r="G183" s="20" t="n">
@@ -11441,7 +11441,7 @@
         <v>16</v>
       </c>
       <c r="F184" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B184, C184, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B184, C184, holiday!A$2:A$499)</f>
         <v>11</v>
       </c>
       <c r="G184" s="20" t="n">
@@ -11487,7 +11487,7 @@
         <v>111</v>
       </c>
       <c r="F185" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B185, C185, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B185, C185, holiday!A$2:A$499)</f>
         <v>79</v>
       </c>
       <c r="G185" s="20" t="n">
@@ -11533,7 +11533,7 @@
         <v>16</v>
       </c>
       <c r="F186" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B186, C186, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B186, C186, holiday!A$2:A$499)</f>
         <v>10</v>
       </c>
       <c r="G186" s="20" t="n">
@@ -11579,20 +11579,20 @@
         <v>91</v>
       </c>
       <c r="F187" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B187, C187, holiday!A$2:A$500)</f>
-        <v>64</v>
+        <f aca="false">NETWORKDAYS(B187, C187, holiday!A$2:A$499)</f>
+        <v>65</v>
       </c>
       <c r="G187" s="20" t="n">
         <f aca="false">D187/F187</f>
-        <v>7.03125</v>
+        <v>6.92307692307692</v>
       </c>
       <c r="H187" s="21" t="n">
         <f aca="false">_xlfn.FLOOR.MATH(G187, 0.25)</f>
-        <v>7</v>
+        <v>6.75</v>
       </c>
       <c r="I187" s="21" t="n">
         <f aca="false">H187 + 0.25</f>
-        <v>7.25</v>
+        <v>7</v>
       </c>
       <c r="J187" s="2" t="b">
         <f aca="false">COUNTIF(assign!$B$1:$B$563, A187) &gt; 0</f>
@@ -11625,7 +11625,7 @@
         <v>31</v>
       </c>
       <c r="F188" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B188, C188, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B188, C188, holiday!A$2:A$499)</f>
         <v>22</v>
       </c>
       <c r="G188" s="20" t="n">
@@ -11671,12 +11671,12 @@
         <v>171</v>
       </c>
       <c r="F189" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B189, C189, holiday!A$2:A$500)</f>
-        <v>121</v>
+        <f aca="false">NETWORKDAYS(B189, C189, holiday!A$2:A$499)</f>
+        <v>122</v>
       </c>
       <c r="G189" s="20" t="n">
         <f aca="false">D189/F189</f>
-        <v>5.37190082644628</v>
+        <v>5.32786885245902</v>
       </c>
       <c r="H189" s="21" t="n">
         <f aca="false">_xlfn.FLOOR.MATH(G189, 0.25)</f>
@@ -11717,7 +11717,7 @@
         <v>46</v>
       </c>
       <c r="F190" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B190, C190, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B190, C190, holiday!A$2:A$499)</f>
         <v>32</v>
       </c>
       <c r="G190" s="20" t="n">
@@ -11763,20 +11763,20 @@
         <v>156</v>
       </c>
       <c r="F191" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B191, C191, holiday!A$2:A$500)</f>
-        <v>110</v>
+        <f aca="false">NETWORKDAYS(B191, C191, holiday!A$2:A$499)</f>
+        <v>111</v>
       </c>
       <c r="G191" s="20" t="n">
         <f aca="false">D191/F191</f>
-        <v>7.27272727272727</v>
+        <v>7.20720720720721</v>
       </c>
       <c r="H191" s="21" t="n">
         <f aca="false">_xlfn.FLOOR.MATH(G191, 0.25)</f>
-        <v>7.25</v>
+        <v>7</v>
       </c>
       <c r="I191" s="21" t="n">
         <f aca="false">H191 + 0.25</f>
-        <v>7.5</v>
+        <v>7.25</v>
       </c>
       <c r="J191" s="2" t="b">
         <f aca="false">COUNTIF(assign!$B$1:$B$563, A191) &gt; 0</f>
@@ -11809,7 +11809,7 @@
         <v>31</v>
       </c>
       <c r="F192" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B192, C192, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B192, C192, holiday!A$2:A$499)</f>
         <v>21</v>
       </c>
       <c r="G192" s="20" t="n">
@@ -11855,12 +11855,12 @@
         <v>56</v>
       </c>
       <c r="F193" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B193, C193, holiday!A$2:A$500)</f>
-        <v>39</v>
+        <f aca="false">NETWORKDAYS(B193, C193, holiday!A$2:A$499)</f>
+        <v>40</v>
       </c>
       <c r="G193" s="20" t="n">
         <f aca="false">D193/F193</f>
-        <v>5.64102564102564</v>
+        <v>5.5</v>
       </c>
       <c r="H193" s="21" t="n">
         <f aca="false">_xlfn.FLOOR.MATH(G193, 0.25)</f>
@@ -11901,7 +11901,7 @@
         <v>46</v>
       </c>
       <c r="F194" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B194, C194, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B194, C194, holiday!A$2:A$499)</f>
         <v>33</v>
       </c>
       <c r="G194" s="20" t="n">
@@ -11947,20 +11947,20 @@
         <v>74</v>
       </c>
       <c r="F195" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B195, C195, holiday!A$2:A$500)</f>
-        <v>52</v>
+        <f aca="false">NETWORKDAYS(B195, C195, holiday!A$2:A$499)</f>
+        <v>53</v>
       </c>
       <c r="G195" s="20" t="n">
         <f aca="false">D195/F195</f>
-        <v>4.80769230769231</v>
+        <v>4.71698113207547</v>
       </c>
       <c r="H195" s="21" t="n">
         <f aca="false">_xlfn.FLOOR.MATH(G195, 0.25)</f>
-        <v>4.75</v>
+        <v>4.5</v>
       </c>
       <c r="I195" s="21" t="n">
         <f aca="false">H195 + 0.25</f>
-        <v>5</v>
+        <v>4.75</v>
       </c>
       <c r="J195" s="2" t="b">
         <f aca="false">COUNTIF(assign!$B$1:$B$563, A195) &gt; 0</f>
@@ -11993,7 +11993,7 @@
         <v>46</v>
       </c>
       <c r="F196" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B196, C196, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B196, C196, holiday!A$2:A$499)</f>
         <v>32</v>
       </c>
       <c r="G196" s="20" t="n">
@@ -12039,12 +12039,12 @@
         <v>91</v>
       </c>
       <c r="F197" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B197, C197, holiday!A$2:A$500)</f>
-        <v>64</v>
+        <f aca="false">NETWORKDAYS(B197, C197, holiday!A$2:A$499)</f>
+        <v>65</v>
       </c>
       <c r="G197" s="20" t="n">
         <f aca="false">D197/F197</f>
-        <v>2.34375</v>
+        <v>2.30769230769231</v>
       </c>
       <c r="H197" s="21" t="n">
         <f aca="false">_xlfn.FLOOR.MATH(G197, 0.25)</f>
@@ -12085,7 +12085,7 @@
         <v>31</v>
       </c>
       <c r="F198" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B198, C198, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B198, C198, holiday!A$2:A$499)</f>
         <v>22</v>
       </c>
       <c r="G198" s="20" t="n">
@@ -12131,12 +12131,12 @@
         <v>132</v>
       </c>
       <c r="F199" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B199, C199, holiday!A$2:A$500)</f>
-        <v>92</v>
+        <f aca="false">NETWORKDAYS(B199, C199, holiday!A$2:A$499)</f>
+        <v>93</v>
       </c>
       <c r="G199" s="20" t="n">
         <f aca="false">D199/F199</f>
-        <v>3.80434782608696</v>
+        <v>3.76344086021505</v>
       </c>
       <c r="H199" s="21" t="n">
         <f aca="false">_xlfn.FLOOR.MATH(G199, 0.25)</f>
@@ -12177,7 +12177,7 @@
         <v>46</v>
       </c>
       <c r="F200" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B200, C200, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B200, C200, holiday!A$2:A$499)</f>
         <v>34</v>
       </c>
       <c r="G200" s="20" t="n">
@@ -12223,12 +12223,12 @@
         <v>244</v>
       </c>
       <c r="F201" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B201, C201, holiday!A$2:A$500)</f>
-        <v>172</v>
+        <f aca="false">NETWORKDAYS(B201, C201, holiday!A$2:A$499)</f>
+        <v>173</v>
       </c>
       <c r="G201" s="20" t="n">
         <f aca="false">D201/F201</f>
-        <v>4.36046511627907</v>
+        <v>4.33526011560694</v>
       </c>
       <c r="H201" s="21" t="n">
         <f aca="false">_xlfn.FLOOR.MATH(G201, 0.25)</f>
@@ -12269,7 +12269,7 @@
         <v>46</v>
       </c>
       <c r="F202" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B202, C202, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B202, C202, holiday!A$2:A$499)</f>
         <v>34</v>
       </c>
       <c r="G202" s="20" t="n">
@@ -12315,12 +12315,12 @@
         <v>274</v>
       </c>
       <c r="F203" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B203, C203, holiday!A$2:A$500)</f>
-        <v>194</v>
+        <f aca="false">NETWORKDAYS(B203, C203, holiday!A$2:A$499)</f>
+        <v>195</v>
       </c>
       <c r="G203" s="20" t="n">
         <f aca="false">D203/F203</f>
-        <v>5.67010309278351</v>
+        <v>5.64102564102564</v>
       </c>
       <c r="H203" s="21" t="n">
         <f aca="false">_xlfn.FLOOR.MATH(G203, 0.25)</f>
@@ -12361,7 +12361,7 @@
         <v>31</v>
       </c>
       <c r="F204" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B204, C204, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B204, C204, holiday!A$2:A$499)</f>
         <v>22</v>
       </c>
       <c r="G204" s="20" t="n">
@@ -12407,7 +12407,7 @@
         <v>18</v>
       </c>
       <c r="F205" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B205, C205, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B205, C205, holiday!A$2:A$499)</f>
         <v>14</v>
       </c>
       <c r="G205" s="20" t="n">
@@ -12453,7 +12453,7 @@
         <v>123</v>
       </c>
       <c r="F206" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B206, C206, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B206, C206, holiday!A$2:A$499)</f>
         <v>86</v>
       </c>
       <c r="G206" s="20" t="n">
@@ -12499,7 +12499,7 @@
         <v>46</v>
       </c>
       <c r="F207" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B207, C207, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B207, C207, holiday!A$2:A$499)</f>
         <v>34</v>
       </c>
       <c r="G207" s="20" t="n">
@@ -12545,7 +12545,7 @@
         <v>24</v>
       </c>
       <c r="F208" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B208, C208, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B208, C208, holiday!A$2:A$499)</f>
         <v>16</v>
       </c>
       <c r="G208" s="20" t="n">
@@ -12591,7 +12591,7 @@
         <v>130</v>
       </c>
       <c r="F209" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B209, C209, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B209, C209, holiday!A$2:A$499)</f>
         <v>93</v>
       </c>
       <c r="G209" s="20" t="n">
@@ -12637,7 +12637,7 @@
         <v>46</v>
       </c>
       <c r="F210" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B210, C210, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B210, C210, holiday!A$2:A$499)</f>
         <v>32</v>
       </c>
       <c r="G210" s="20" t="n">
@@ -12683,7 +12683,7 @@
         <v>30</v>
       </c>
       <c r="F211" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B211, C211, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B211, C211, holiday!A$2:A$499)</f>
         <v>21</v>
       </c>
       <c r="G211" s="20" t="n">
@@ -12729,7 +12729,7 @@
         <v>196</v>
       </c>
       <c r="F212" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B212, C212, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B212, C212, holiday!A$2:A$499)</f>
         <v>139</v>
       </c>
       <c r="G212" s="20" t="n">
@@ -12775,7 +12775,7 @@
         <v>29</v>
       </c>
       <c r="F213" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B213, C213, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B213, C213, holiday!A$2:A$499)</f>
         <v>20</v>
       </c>
       <c r="G213" s="20" t="n">
@@ -12821,7 +12821,7 @@
         <v>11</v>
       </c>
       <c r="F214" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B214, C214, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B214, C214, holiday!A$2:A$499)</f>
         <v>7</v>
       </c>
       <c r="G214" s="20" t="n">
@@ -12867,7 +12867,7 @@
         <v>154</v>
       </c>
       <c r="F215" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B215, C215, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B215, C215, holiday!A$2:A$499)</f>
         <v>109</v>
       </c>
       <c r="G215" s="20" t="n">
@@ -12913,7 +12913,7 @@
         <v>35</v>
       </c>
       <c r="F216" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B216, C216, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B216, C216, holiday!A$2:A$499)</f>
         <v>25</v>
       </c>
       <c r="G216" s="20" t="n">
@@ -12959,7 +12959,7 @@
         <v>20</v>
       </c>
       <c r="F217" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B217, C217, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B217, C217, holiday!A$2:A$499)</f>
         <v>15</v>
       </c>
       <c r="G217" s="20" t="n">
@@ -13005,7 +13005,7 @@
         <v>199</v>
       </c>
       <c r="F218" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B218, C218, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B218, C218, holiday!A$2:A$499)</f>
         <v>142</v>
       </c>
       <c r="G218" s="20" t="n">
@@ -13051,7 +13051,7 @@
         <v>32</v>
       </c>
       <c r="F219" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B219, C219, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B219, C219, holiday!A$2:A$499)</f>
         <v>23</v>
       </c>
       <c r="G219" s="20" t="n">
@@ -13097,7 +13097,7 @@
         <v>15</v>
       </c>
       <c r="F220" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B220, C220, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B220, C220, holiday!A$2:A$499)</f>
         <v>11</v>
       </c>
       <c r="G220" s="20" t="n">
@@ -13143,7 +13143,7 @@
         <v>174</v>
       </c>
       <c r="F221" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B221, C221, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B221, C221, holiday!A$2:A$499)</f>
         <v>124</v>
       </c>
       <c r="G221" s="20" t="n">
@@ -13189,7 +13189,7 @@
         <v>32</v>
       </c>
       <c r="F222" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B222, C222, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B222, C222, holiday!A$2:A$499)</f>
         <v>23</v>
       </c>
       <c r="G222" s="20" t="n">
@@ -13235,7 +13235,7 @@
         <v>6</v>
       </c>
       <c r="F223" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B223, C223, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B223, C223, holiday!A$2:A$499)</f>
         <v>5</v>
       </c>
       <c r="G223" s="20" t="n">
@@ -13281,7 +13281,7 @@
         <v>46</v>
       </c>
       <c r="F224" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B224, C224, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B224, C224, holiday!A$2:A$499)</f>
         <v>33</v>
       </c>
       <c r="G224" s="20" t="n">
@@ -13327,7 +13327,7 @@
         <v>13</v>
       </c>
       <c r="F225" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B225, C225, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B225, C225, holiday!A$2:A$499)</f>
         <v>9</v>
       </c>
       <c r="G225" s="20" t="n">
@@ -13373,7 +13373,7 @@
         <v>11</v>
       </c>
       <c r="F226" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B226, C226, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B226, C226, holiday!A$2:A$499)</f>
         <v>8</v>
       </c>
       <c r="G226" s="20" t="n">
@@ -13419,7 +13419,7 @@
         <v>181</v>
       </c>
       <c r="F227" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B227, C227, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B227, C227, holiday!A$2:A$499)</f>
         <v>128</v>
       </c>
       <c r="G227" s="20" t="n">
@@ -13465,7 +13465,7 @@
         <v>20</v>
       </c>
       <c r="F228" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B228, C228, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B228, C228, holiday!A$2:A$499)</f>
         <v>14</v>
       </c>
       <c r="G228" s="20" t="n">
@@ -13511,12 +13511,12 @@
         <v>171</v>
       </c>
       <c r="F229" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B229, C229, holiday!A$2:A$500)</f>
-        <v>121</v>
+        <f aca="false">NETWORKDAYS(B229, C229, holiday!A$2:A$499)</f>
+        <v>122</v>
       </c>
       <c r="G229" s="20" t="n">
         <f aca="false">D229/F229</f>
-        <v>2.39669421487603</v>
+        <v>2.37704918032787</v>
       </c>
       <c r="H229" s="21" t="n">
         <f aca="false">_xlfn.FLOOR.MATH(G229, 0.25)</f>
@@ -13557,7 +13557,7 @@
         <v>11</v>
       </c>
       <c r="F230" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B230, C230, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B230, C230, holiday!A$2:A$499)</f>
         <v>7</v>
       </c>
       <c r="G230" s="20" t="n">
@@ -13603,20 +13603,20 @@
         <v>21</v>
       </c>
       <c r="F231" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B231, C231, holiday!A$2:A$500)</f>
-        <v>14</v>
+        <f aca="false">NETWORKDAYS(B231, C231, holiday!A$2:A$499)</f>
+        <v>15</v>
       </c>
       <c r="G231" s="20" t="n">
         <f aca="false">D231/F231</f>
-        <v>12.8571428571429</v>
+        <v>12</v>
       </c>
       <c r="H231" s="21" t="n">
         <f aca="false">_xlfn.FLOOR.MATH(G231, 0.25)</f>
-        <v>12.75</v>
+        <v>12</v>
       </c>
       <c r="I231" s="21" t="n">
         <f aca="false">H231 + 0.25</f>
-        <v>13</v>
+        <v>12.25</v>
       </c>
       <c r="J231" s="2" t="b">
         <f aca="false">COUNTIF(assign!$B$1:$B$563, A231) &gt; 0</f>
@@ -13649,7 +13649,7 @@
         <v>48</v>
       </c>
       <c r="F232" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B232, C232, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B232, C232, holiday!A$2:A$499)</f>
         <v>34</v>
       </c>
       <c r="G232" s="20" t="n">
@@ -13696,12 +13696,12 @@
         <v>81</v>
       </c>
       <c r="F233" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B233, C233, holiday!A$2:A$500)</f>
-        <v>57</v>
+        <f aca="false">NETWORKDAYS(B233, C233, holiday!A$2:A$499)</f>
+        <v>58</v>
       </c>
       <c r="G233" s="20" t="n">
         <f aca="false">D233/F233</f>
-        <v>1.57894736842105</v>
+        <v>1.55172413793103</v>
       </c>
       <c r="H233" s="21" t="n">
         <f aca="false">_xlfn.FLOOR.MATH(G233, 0.25)</f>
@@ -13743,7 +13743,7 @@
         <v>10</v>
       </c>
       <c r="F234" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B234, C234, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B234, C234, holiday!A$2:A$499)</f>
         <v>7</v>
       </c>
       <c r="G234" s="20" t="n">
@@ -13789,20 +13789,20 @@
         <v>21</v>
       </c>
       <c r="F235" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B235, C235, holiday!A$2:A$500)</f>
-        <v>14</v>
+        <f aca="false">NETWORKDAYS(B235, C235, holiday!A$2:A$499)</f>
+        <v>15</v>
       </c>
       <c r="G235" s="20" t="n">
         <f aca="false">D235/F235</f>
-        <v>10.7142857142857</v>
+        <v>10</v>
       </c>
       <c r="H235" s="21" t="n">
         <f aca="false">_xlfn.FLOOR.MATH(G235, 0.25)</f>
-        <v>10.5</v>
+        <v>10</v>
       </c>
       <c r="I235" s="21" t="n">
         <f aca="false">H235 + 0.25</f>
-        <v>10.75</v>
+        <v>10.25</v>
       </c>
       <c r="J235" s="2" t="b">
         <f aca="false">COUNTIF(assign!$B$1:$B$563, A235) &gt; 0</f>
@@ -13835,7 +13835,7 @@
         <v>13</v>
       </c>
       <c r="F236" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B236, C236, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B236, C236, holiday!A$2:A$499)</f>
         <v>9</v>
       </c>
       <c r="G236" s="20" t="n">
@@ -13881,20 +13881,20 @@
         <v>81</v>
       </c>
       <c r="F237" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B237, C237, holiday!A$2:A$500)</f>
-        <v>57</v>
+        <f aca="false">NETWORKDAYS(B237, C237, holiday!A$2:A$499)</f>
+        <v>58</v>
       </c>
       <c r="G237" s="20" t="n">
         <f aca="false">D237/F237</f>
-        <v>7.01754385964912</v>
+        <v>6.89655172413793</v>
       </c>
       <c r="H237" s="21" t="n">
         <f aca="false">_xlfn.FLOOR.MATH(G237, 0.25)</f>
-        <v>7</v>
+        <v>6.75</v>
       </c>
       <c r="I237" s="21" t="n">
         <f aca="false">H237 + 0.25</f>
-        <v>7.25</v>
+        <v>7</v>
       </c>
       <c r="J237" s="2" t="b">
         <f aca="false">COUNTIF(assign!$B$1:$B$563, A237) &gt; 0</f>
@@ -13927,7 +13927,7 @@
         <v>9</v>
       </c>
       <c r="F238" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B238, C238, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B238, C238, holiday!A$2:A$499)</f>
         <v>6</v>
       </c>
       <c r="G238" s="20" t="n">
@@ -13973,12 +13973,12 @@
         <v>46</v>
       </c>
       <c r="F239" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B239, C239, holiday!A$2:A$500)</f>
-        <v>32</v>
+        <f aca="false">NETWORKDAYS(B239, C239, holiday!A$2:A$499)</f>
+        <v>33</v>
       </c>
       <c r="G239" s="20" t="n">
         <f aca="false">D239/F239</f>
-        <v>5.15625</v>
+        <v>5</v>
       </c>
       <c r="H239" s="21" t="n">
         <f aca="false">_xlfn.FLOOR.MATH(G239, 0.25)</f>
@@ -14019,7 +14019,7 @@
         <v>10</v>
       </c>
       <c r="F240" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B240, C240, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B240, C240, holiday!A$2:A$499)</f>
         <v>7</v>
       </c>
       <c r="G240" s="20" t="n">
@@ -14065,12 +14065,12 @@
         <v>76</v>
       </c>
       <c r="F241" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B241, C241, holiday!A$2:A$500)</f>
-        <v>53</v>
+        <f aca="false">NETWORKDAYS(B241, C241, holiday!A$2:A$499)</f>
+        <v>54</v>
       </c>
       <c r="G241" s="20" t="n">
         <f aca="false">D241/F241</f>
-        <v>6.9811320754717</v>
+        <v>6.85185185185185</v>
       </c>
       <c r="H241" s="21" t="n">
         <f aca="false">_xlfn.FLOOR.MATH(G241, 0.25)</f>
@@ -14111,7 +14111,7 @@
         <v>8</v>
       </c>
       <c r="F242" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B242, C242, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B242, C242, holiday!A$2:A$499)</f>
         <v>6</v>
       </c>
       <c r="G242" s="20" t="n">
@@ -14158,20 +14158,20 @@
         <v>81</v>
       </c>
       <c r="F243" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B243, C243, holiday!A$2:A$500)</f>
-        <v>57</v>
+        <f aca="false">NETWORKDAYS(B243, C243, holiday!A$2:A$499)</f>
+        <v>58</v>
       </c>
       <c r="G243" s="20" t="n">
         <f aca="false">D243/F243</f>
-        <v>8.7719298245614</v>
+        <v>8.62068965517242</v>
       </c>
       <c r="H243" s="21" t="n">
         <f aca="false">_xlfn.FLOOR.MATH(G243, 0.25)</f>
-        <v>8.75</v>
+        <v>8.5</v>
       </c>
       <c r="I243" s="21" t="n">
         <f aca="false">H243 + 0.25</f>
-        <v>9</v>
+        <v>8.75</v>
       </c>
       <c r="J243" s="2" t="b">
         <f aca="false">COUNTIF(assign!$B$1:$B$563, A243) &gt; 0</f>
@@ -14205,7 +14205,7 @@
         <v>10</v>
       </c>
       <c r="F244" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B244, C244, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B244, C244, holiday!A$2:A$499)</f>
         <v>7</v>
       </c>
       <c r="G244" s="20" t="n">
@@ -14252,12 +14252,12 @@
         <v>56</v>
       </c>
       <c r="F245" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B245, C245, holiday!A$2:A$500)</f>
-        <v>39</v>
+        <f aca="false">NETWORKDAYS(B245, C245, holiday!A$2:A$499)</f>
+        <v>40</v>
       </c>
       <c r="G245" s="20" t="n">
         <f aca="false">D245/F245</f>
-        <v>7.69230769230769</v>
+        <v>7.5</v>
       </c>
       <c r="H245" s="21" t="n">
         <f aca="false">_xlfn.FLOOR.MATH(G245, 0.25)</f>
@@ -14299,7 +14299,7 @@
         <v>6</v>
       </c>
       <c r="F246" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B246, C246, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B246, C246, holiday!A$2:A$499)</f>
         <v>4</v>
       </c>
       <c r="G246" s="20" t="n">
@@ -14345,12 +14345,12 @@
         <v>56</v>
       </c>
       <c r="F247" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B247, C247, holiday!A$2:A$500)</f>
-        <v>39</v>
+        <f aca="false">NETWORKDAYS(B247, C247, holiday!A$2:A$499)</f>
+        <v>40</v>
       </c>
       <c r="G247" s="20" t="n">
         <f aca="false">D247/F247</f>
-        <v>6.41025641025641</v>
+        <v>6.25</v>
       </c>
       <c r="H247" s="21" t="n">
         <f aca="false">_xlfn.FLOOR.MATH(G247, 0.25)</f>
@@ -14391,7 +14391,7 @@
         <v>6</v>
       </c>
       <c r="F248" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B248, C248, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B248, C248, holiday!A$2:A$499)</f>
         <v>4</v>
       </c>
       <c r="G248" s="20" t="n">
@@ -14438,7 +14438,7 @@
         <v>16</v>
       </c>
       <c r="F249" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B249, C249, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B249, C249, holiday!A$2:A$499)</f>
         <v>11</v>
       </c>
       <c r="G249" s="20" t="n">
@@ -14486,7 +14486,7 @@
         <v>111</v>
       </c>
       <c r="F250" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B250, C250, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B250, C250, holiday!A$2:A$499)</f>
         <v>79</v>
       </c>
       <c r="G250" s="20" t="n">
@@ -14533,7 +14533,7 @@
         <v>16</v>
       </c>
       <c r="F251" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B251, C251, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B251, C251, holiday!A$2:A$499)</f>
         <v>10</v>
       </c>
       <c r="G251" s="20" t="n">
@@ -14579,20 +14579,20 @@
         <v>86</v>
       </c>
       <c r="F252" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B252, C252, holiday!A$2:A$500)</f>
-        <v>61</v>
+        <f aca="false">NETWORKDAYS(B252, C252, holiday!A$2:A$499)</f>
+        <v>62</v>
       </c>
       <c r="G252" s="20" t="n">
         <f aca="false">D252/F252</f>
-        <v>9.83606557377049</v>
+        <v>9.67741935483871</v>
       </c>
       <c r="H252" s="21" t="n">
         <f aca="false">_xlfn.FLOOR.MATH(G252, 0.25)</f>
-        <v>9.75</v>
+        <v>9.5</v>
       </c>
       <c r="I252" s="21" t="n">
         <f aca="false">H252 + 0.25</f>
-        <v>10</v>
+        <v>9.75</v>
       </c>
       <c r="J252" s="2" t="b">
         <f aca="false">COUNTIF(assign!$B$1:$B$563, A252) &gt; 0</f>
@@ -14625,7 +14625,7 @@
         <v>11</v>
       </c>
       <c r="F253" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B253, C253, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B253, C253, holiday!A$2:A$499)</f>
         <v>7</v>
       </c>
       <c r="G253" s="20" t="n">
@@ -14671,12 +14671,12 @@
         <v>171</v>
       </c>
       <c r="F254" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B254, C254, holiday!A$2:A$500)</f>
-        <v>121</v>
+        <f aca="false">NETWORKDAYS(B254, C254, holiday!A$2:A$499)</f>
+        <v>122</v>
       </c>
       <c r="G254" s="20" t="n">
         <f aca="false">D254/F254</f>
-        <v>4.62809917355372</v>
+        <v>4.59016393442623</v>
       </c>
       <c r="H254" s="21" t="n">
         <f aca="false">_xlfn.FLOOR.MATH(G254, 0.25)</f>
@@ -14717,7 +14717,7 @@
         <v>10</v>
       </c>
       <c r="F255" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B255, C255, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B255, C255, holiday!A$2:A$499)</f>
         <v>6</v>
       </c>
       <c r="G255" s="20" t="n">
@@ -14763,12 +14763,12 @@
         <v>171</v>
       </c>
       <c r="F256" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B256, C256, holiday!A$2:A$500)</f>
-        <v>121</v>
+        <f aca="false">NETWORKDAYS(B256, C256, holiday!A$2:A$499)</f>
+        <v>122</v>
       </c>
       <c r="G256" s="20" t="n">
         <f aca="false">D256/F256</f>
-        <v>6.61157024793388</v>
+        <v>6.55737704918033</v>
       </c>
       <c r="H256" s="21" t="n">
         <f aca="false">_xlfn.FLOOR.MATH(G256, 0.25)</f>
@@ -14809,7 +14809,7 @@
         <v>10</v>
       </c>
       <c r="F257" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B257, C257, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B257, C257, holiday!A$2:A$499)</f>
         <v>6</v>
       </c>
       <c r="G257" s="20" t="n">
@@ -14855,7 +14855,7 @@
         <v>26</v>
       </c>
       <c r="F258" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B258, C258, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B258, C258, holiday!A$2:A$499)</f>
         <v>19</v>
       </c>
       <c r="G258" s="20" t="n">
@@ -14901,7 +14901,7 @@
         <v>501</v>
       </c>
       <c r="F259" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B259, C259, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B259, C259, holiday!A$2:A$499)</f>
         <v>357</v>
       </c>
       <c r="G259" s="20" t="n">
@@ -14947,7 +14947,7 @@
         <v>56</v>
       </c>
       <c r="F260" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B260, C260, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B260, C260, holiday!A$2:A$499)</f>
         <v>40</v>
       </c>
       <c r="G260" s="20" t="n">
@@ -14993,12 +14993,12 @@
         <v>141</v>
       </c>
       <c r="F261" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B261, C261, holiday!A$2:A$500)</f>
-        <v>99</v>
+        <f aca="false">NETWORKDAYS(B261, C261, holiday!A$2:A$499)</f>
+        <v>100</v>
       </c>
       <c r="G261" s="20" t="n">
         <f aca="false">D261/F261</f>
-        <v>3.03030303030303</v>
+        <v>3</v>
       </c>
       <c r="H261" s="21" t="n">
         <f aca="false">_xlfn.FLOOR.MATH(G261, 0.25)</f>
@@ -15039,7 +15039,7 @@
         <v>12</v>
       </c>
       <c r="F262" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B262, C262, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B262, C262, holiday!A$2:A$499)</f>
         <v>8</v>
       </c>
       <c r="G262" s="20" t="n">
@@ -15085,20 +15085,20 @@
         <v>61</v>
       </c>
       <c r="F263" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B263, C263, holiday!A$2:A$500)</f>
-        <v>42</v>
+        <f aca="false">NETWORKDAYS(B263, C263, holiday!A$2:A$499)</f>
+        <v>43</v>
       </c>
       <c r="G263" s="20" t="n">
         <f aca="false">D263/F263</f>
-        <v>7.85714285714286</v>
+        <v>7.67441860465116</v>
       </c>
       <c r="H263" s="21" t="n">
         <f aca="false">_xlfn.FLOOR.MATH(G263, 0.25)</f>
-        <v>7.75</v>
+        <v>7.5</v>
       </c>
       <c r="I263" s="21" t="n">
         <f aca="false">H263 + 0.25</f>
-        <v>8</v>
+        <v>7.75</v>
       </c>
       <c r="J263" s="2" t="b">
         <f aca="false">COUNTIF(assign!$B$1:$B$563, A263) &gt; 0</f>
@@ -15131,7 +15131,7 @@
         <v>8</v>
       </c>
       <c r="F264" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B264, C264, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B264, C264, holiday!A$2:A$499)</f>
         <v>6</v>
       </c>
       <c r="G264" s="20" t="n">
@@ -15177,7 +15177,7 @@
         <v>15</v>
       </c>
       <c r="F265" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B265, C265, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B265, C265, holiday!A$2:A$499)</f>
         <v>11</v>
       </c>
       <c r="G265" s="20" t="n">
@@ -15223,7 +15223,7 @@
         <v>168</v>
       </c>
       <c r="F266" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B266, C266, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B266, C266, holiday!A$2:A$499)</f>
         <v>119</v>
       </c>
       <c r="G266" s="20" t="n">
@@ -15269,7 +15269,7 @@
         <v>16</v>
       </c>
       <c r="F267" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B267, C267, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B267, C267, holiday!A$2:A$499)</f>
         <v>12</v>
       </c>
       <c r="G267" s="20" t="n">
@@ -15315,7 +15315,7 @@
         <v>16</v>
       </c>
       <c r="F268" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B268, C268, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B268, C268, holiday!A$2:A$499)</f>
         <v>11</v>
       </c>
       <c r="G268" s="20" t="n">
@@ -15361,7 +15361,7 @@
         <v>271</v>
       </c>
       <c r="F269" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B269, C269, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B269, C269, holiday!A$2:A$499)</f>
         <v>193</v>
       </c>
       <c r="G269" s="20" t="n">
@@ -15407,7 +15407,7 @@
         <v>19</v>
       </c>
       <c r="F270" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B270, C270, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B270, C270, holiday!A$2:A$499)</f>
         <v>13</v>
       </c>
       <c r="G270" s="20" t="n">
@@ -15453,7 +15453,7 @@
         <v>16</v>
       </c>
       <c r="F271" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B271, C271, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B271, C271, holiday!A$2:A$499)</f>
         <v>10</v>
       </c>
       <c r="G271" s="20" t="n">
@@ -15499,7 +15499,7 @@
         <v>171</v>
       </c>
       <c r="F272" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B272, C272, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B272, C272, holiday!A$2:A$499)</f>
         <v>122</v>
       </c>
       <c r="G272" s="20" t="n">
@@ -15545,7 +15545,7 @@
         <v>12</v>
       </c>
       <c r="F273" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B273, C273, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B273, C273, holiday!A$2:A$499)</f>
         <v>8</v>
       </c>
       <c r="G273" s="20" t="n">
@@ -15591,7 +15591,7 @@
         <v>16</v>
       </c>
       <c r="F274" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B274, C274, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B274, C274, holiday!A$2:A$499)</f>
         <v>12</v>
       </c>
       <c r="G274" s="20" t="n">
@@ -15637,7 +15637,7 @@
         <v>271</v>
       </c>
       <c r="F275" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B275, C275, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B275, C275, holiday!A$2:A$499)</f>
         <v>193</v>
       </c>
       <c r="G275" s="20" t="n">
@@ -15683,7 +15683,7 @@
         <v>23</v>
       </c>
       <c r="F276" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B276, C276, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B276, C276, holiday!A$2:A$499)</f>
         <v>17</v>
       </c>
       <c r="G276" s="20" t="n">
@@ -15729,7 +15729,7 @@
         <v>26</v>
       </c>
       <c r="F277" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B277, C277, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B277, C277, holiday!A$2:A$499)</f>
         <v>19</v>
       </c>
       <c r="G277" s="20" t="n">
@@ -15775,7 +15775,7 @@
         <v>151</v>
       </c>
       <c r="F278" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B278, C278, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B278, C278, holiday!A$2:A$499)</f>
         <v>108</v>
       </c>
       <c r="G278" s="20" t="n">
@@ -15821,7 +15821,7 @@
         <v>25</v>
       </c>
       <c r="F279" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B279, C279, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B279, C279, holiday!A$2:A$499)</f>
         <v>17</v>
       </c>
       <c r="G279" s="20" t="n">
@@ -15867,7 +15867,7 @@
         <v>31</v>
       </c>
       <c r="F280" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B280, C280, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B280, C280, holiday!A$2:A$499)</f>
         <v>22</v>
       </c>
       <c r="G280" s="20" t="n">
@@ -15913,7 +15913,7 @@
         <v>131</v>
       </c>
       <c r="F281" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B281, C281, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B281, C281, holiday!A$2:A$499)</f>
         <v>93</v>
       </c>
       <c r="G281" s="20" t="n">
@@ -15959,7 +15959,7 @@
         <v>8</v>
       </c>
       <c r="F282" s="19" t="n">
-        <f aca="false">NETWORKDAYS(B282, C282, holiday!A$2:A$500)</f>
+        <f aca="false">NETWORKDAYS(B282, C282, holiday!A$2:A$499)</f>
         <v>6</v>
       </c>
       <c r="G282" s="20" t="n">
@@ -25996,11 +25996,11 @@
       </c>
       <c r="E87" s="27" t="n">
         <f aca="false">VLOOKUP(B87, task!A$2:I$300, 8, 0)</f>
-        <v>0.75</v>
+        <v>0.5</v>
       </c>
       <c r="F87" s="27" t="n">
         <f aca="false">VLOOKUP(B87, task!A$2:I$300, 9, 0)</f>
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="G87" s="2" t="b">
         <f aca="false">COUNTIF(expert!$A$2:$A$949, A87) &gt; 0</f>
@@ -41255,10 +41255,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B46"/>
+  <dimension ref="A1:B1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J18" activeCellId="0" sqref="J18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -41272,22 +41272,22 @@
         <v>348</v>
       </c>
       <c r="B1" s="18" t="b">
-        <f aca="false">AND(B2:B905)</f>
-        <v>0</v>
+        <f aca="false">AND(B2:B904)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="n">
-        <v>45658</v>
+        <v>45767</v>
       </c>
       <c r="B2" s="2" t="b">
         <f aca="false">AND(ISNUMBER(A2), misc!$A$2&lt;=A2)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="n">
-        <v>45767</v>
+        <v>45778</v>
       </c>
       <c r="B3" s="2" t="b">
         <f aca="false">AND(ISNUMBER(A3), misc!$A$2&lt;=A3)</f>
@@ -41295,13 +41295,7 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="7" t="n">
-        <v>45778</v>
-      </c>
-      <c r="B4" s="2" t="b">
-        <f aca="false">AND(ISNUMBER(A4), misc!$A$2&lt;=A4)</f>
-        <v>1</v>
-      </c>
+      <c r="A4" s="7"/>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="7"/>
@@ -41426,9 +41420,7 @@
     <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="7"/>
     </row>
-    <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="7"/>
-    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>